<commit_message>
Continue refactoring, building pipeline
</commit_message>
<xml_diff>
--- a/experiment/Journal.xlsx
+++ b/experiment/Journal.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14000" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14000" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Parameters" sheetId="1" r:id="rId1"/>
+    <sheet name="Time + Size" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="34">
   <si>
     <t>ID</t>
   </si>
@@ -109,6 +110,18 @@
   </si>
   <si>
     <t>1MB</t>
+  </si>
+  <si>
+    <t>WSD</t>
+  </si>
+  <si>
+    <t>model</t>
+  </si>
+  <si>
+    <t>context window</t>
+  </si>
+  <si>
+    <t>argmax_i(prod_k(cossim(s_i,c_k))))</t>
   </si>
 </sst>
 </file>
@@ -590,10 +603,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A4:O7"/>
+  <dimension ref="A4:Q7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M15" sqref="M15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -605,9 +618,11 @@
     <col min="10" max="10" width="14.83203125" customWidth="1"/>
     <col min="14" max="14" width="14.33203125" customWidth="1"/>
     <col min="15" max="15" width="16" customWidth="1"/>
+    <col min="16" max="16" width="14.33203125" customWidth="1"/>
+    <col min="17" max="17" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:17">
       <c r="B4" s="3" t="s">
         <v>7</v>
       </c>
@@ -634,8 +649,12 @@
       <c r="O4" s="13" t="s">
         <v>26</v>
       </c>
+      <c r="P4" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q4" s="5"/>
     </row>
-    <row r="5" spans="1:15">
+    <row r="5" spans="1:17">
       <c r="A5" s="2" t="s">
         <v>0</v>
       </c>
@@ -681,8 +700,14 @@
       <c r="O5" s="1" t="s">
         <v>27</v>
       </c>
+      <c r="P5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q5" s="1" t="s">
+        <v>32</v>
+      </c>
     </row>
-    <row r="6" spans="1:15">
+    <row r="6" spans="1:17">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -725,8 +750,14 @@
       <c r="O6">
         <v>100</v>
       </c>
+      <c r="P6" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q6">
+        <v>10</v>
+      </c>
     </row>
-    <row r="7" spans="1:15">
+    <row r="7" spans="1:17">
       <c r="A7" t="s">
         <v>28</v>
       </c>
@@ -750,12 +781,42 @@
       </c>
       <c r="I7">
         <v>200</v>
+      </c>
+      <c r="J7" t="s">
+        <v>24</v>
+      </c>
+      <c r="K7">
+        <v>200</v>
+      </c>
+      <c r="L7">
+        <v>200</v>
+      </c>
+      <c r="M7">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>